<commit_message>
Complete Manager Module Followed by DDF and POM Structure
</commit_message>
<xml_diff>
--- a/src/test/java/com/guru99BankingDemo/testData/Data.xlsx
+++ b/src/test/java/com/guru99BankingDemo/testData/Data.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23805" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="6540" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ManagerRegistrationData" sheetId="2" r:id="rId1"/>
+    <sheet name="ManagerLoginData" sheetId="4" r:id="rId2"/>
+    <sheet name="NewCustthgtryomerData" sheetId="5" r:id="rId3"/>
+    <sheet name="newData" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:X35"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,71 +23,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>mngr314394</t>
-  </si>
-  <si>
-    <t>ujEhEva</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>customerId</t>
-  </si>
-  <si>
-    <t>customerpass</t>
-  </si>
-  <si>
-    <t>Account Id</t>
-  </si>
-  <si>
-    <t>Base Url</t>
-  </si>
-  <si>
-    <t>http://demo.guru99.com/V4/</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="35">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>mngr318118</t>
+  </si>
+  <si>
+    <t>nEzaduq</t>
+  </si>
+  <si>
+    <t>nEzaduq5424</t>
+  </si>
+  <si>
+    <t>nEzadufvd</t>
+  </si>
+  <si>
+    <t>nEzaduqu</t>
+  </si>
+  <si>
+    <t>mngr39879846343</t>
+  </si>
+  <si>
+    <t>&lt;*&amp;.com</t>
+  </si>
+  <si>
+    <t>56@gmail.com</t>
+  </si>
+  <si>
+    <t>ewdrfe89798778@.vim</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Date Of Birth(Month)</t>
+  </si>
+  <si>
+    <t>Date Of Birth(Day)</t>
+  </si>
+  <si>
+    <t>Date Of Birth(Year)</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Auntor</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>pathrail</t>
+  </si>
+  <si>
+    <t>Tangail</t>
+  </si>
+  <si>
+    <t>dhaka</t>
+  </si>
+  <si>
+    <t>achar@gmail.com</t>
+  </si>
+  <si>
+    <t>12345##abc</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>sdigdskjidk</t>
+  </si>
+  <si>
+    <t>4445@45#dfg</t>
+  </si>
+  <si>
+    <t>ac9dd19r@gmail.com</t>
+  </si>
+  <si>
+    <t>dfvdf74774d@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,8 +150,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -120,7 +179,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,53 +208,67 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,98 +581,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25">
+    <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="39" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="23.25">
+      <c r="M1" s="9"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J2" s="6">
+        <v>747114589</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="23.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="23.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="23.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="23.25">
-      <c r="A7" s="6">
-        <v>51972</v>
-      </c>
-      <c r="B7" s="7">
-        <v>12345</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="23.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="23.25">
-      <c r="A11" s="6">
-        <v>90562</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="23.25">
-      <c r="A13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6">
+        <v>12123</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" customFormat="1">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1212345</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" customFormat="1">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" customFormat="1">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" customFormat="1">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="6">
+        <v>123456</v>
+      </c>
+      <c r="I8" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" customFormat="1">
+      <c r="A9" s="6">
+        <v>522</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" customFormat="1">
+      <c r="A10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="6">
+        <v>123456</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" customFormat="1">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" customFormat="1"/>
+    <row r="13" spans="1:14" customFormat="1"/>
+    <row r="14" spans="1:14" customFormat="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K4" r:id="rId2"/>
+    <hyperlink ref="K5" r:id="rId3"/>
+    <hyperlink ref="K6" r:id="rId4"/>
+    <hyperlink ref="K7" r:id="rId5"/>
+    <hyperlink ref="K8" r:id="rId6"/>
+    <hyperlink ref="K9" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId8"/>
+    <hyperlink ref="K11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="10" max="10" width="28.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6">
+        <v>191212</v>
+      </c>
+      <c r="J2" s="6">
+        <v>54614521</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1998</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6">
+        <v>12123</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1795486253</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>